<commit_message>
updated code details file
</commit_message>
<xml_diff>
--- a/Code_Details.xlsx
+++ b/Code_Details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usama\DriveShare\NLP\Projects\End_to_End_Projects\DVC-NLP-project-docs-template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19C4E378-C619-4532-8E03-5ACD19D912E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B3E6264-C958-4C05-BF58-D14C9D216596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14085" yWindow="1890" windowWidth="16635" windowHeight="13935" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="345" yWindow="900" windowWidth="16635" windowHeight="13935" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>File : data.xml</t>
   </si>
@@ -54,16 +54,483 @@
     <t>STEPS</t>
   </si>
   <si>
-    <t>Create a template in src/stage_01_prepare_data.py</t>
-  </si>
-  <si>
     <t>Give stage name within template "Prepare_data"</t>
   </si>
   <si>
     <t>In params.yaml present in root directory, we have to give the parameters that will be required in the stages</t>
   </si>
   <si>
-    <t>Let's create stagewise docs in docs folder for better documenation and update that into mkdocs.yml too.</t>
+    <t>Stage 1 : Data Preparation</t>
+  </si>
+  <si>
+    <t>Stage 2 : Data Preparation</t>
+  </si>
+  <si>
+    <t>Give stage name within template "Featurization"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Initial Steps : </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>config/config.yml</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and write the configurations that will be used in project</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create a template in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>src/stage_01_prepare_data.py</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Let's create stagewise docs in docs folder for better documenation and update that into </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>mkdocs.yml</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> too.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Use this function in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>src/stage_01_prepare_data.py</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create a template in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>src/stage_02_featurization.py</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Write a function to create </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>artifacts/prepared</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> folder which will take the dir names from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>config.yml</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> file</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>data_mgmt.py</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> file in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>src/utils</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> folder and write a function to process the data and get train and test split data and save them inside </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>artifacts/prepared</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> folder</t>
+    </r>
+  </si>
+  <si>
+    <t>Keep logging at the end of every function</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>data</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> folder in root directory and put the main data file in it.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create the pages as required in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>docs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> folder in root dir</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">mkdocs reads the pages from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>docs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> folder</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>mkdocs.yml</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and define the interface and details of Documentation</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">docs </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>folder in root dir having</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> javascript/mathjax.js</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> file and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>img</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> folder having images and pages</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> file with .md</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> extension. It will be used by mkdocs for documentation</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>src</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> folder in root dir will have all the stagewise files of project and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>src/utils</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> folder will have functions to be used in stages files</t>
+    </r>
+  </si>
+  <si>
+    <t>we can either use requiremets.txt or conda.yml file for installing dependencies</t>
+  </si>
+  <si>
+    <t>DevOps Part of Project</t>
   </si>
 </sst>
 </file>
@@ -107,10 +574,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -393,80 +865,194 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:B16"/>
+  <dimension ref="B2:B43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="95.42578125" customWidth="1"/>
+    <col min="2" max="2" width="103.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="2:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B16" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="2"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="2"/>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="2"/>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="2"/>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="2"/>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" s="2"/>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" s="2"/>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B37" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B39" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B41" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>11</v>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B42" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B43" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stage 02 function added
</commit_message>
<xml_diff>
--- a/Code_Details.xlsx
+++ b/Code_Details.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usama\DriveShare\NLP\Projects\End_to_End_Projects\DVC-NLP-project-docs-template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usama\Personal\iNeuron\2022\Projects\FSDS-DVC-NLP-project-with-docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA173EC8-5928-42DD-8696-A61A63154099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FE05CF8-57C1-4C78-B805-92418CD1D100}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4680" yWindow="2430" windowWidth="16635" windowHeight="13935" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
   <si>
     <t>File : data.xml</t>
   </si>
@@ -55,9 +55,6 @@
   </si>
   <si>
     <t>Give stage name within template "Prepare_data"</t>
-  </si>
-  <si>
-    <t>In params.yaml present in root directory, we have to give the parameters that will be required in the stages</t>
   </si>
   <si>
     <t>Stage 1 : Data Preparation</t>
@@ -685,13 +682,198 @@
   </si>
   <si>
     <t>CI/CD - For Github Actions:</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">In </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>params.yaml</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> present in root directory, we have to give the parameters that will be required in the data preparation stage</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">As we will be needing dataframe of the required data again and again, so let us create pandas datframe function in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>src/utils/common.py</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">In </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">params.yaml </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>present in root directory, we have to give the parameters that will be required in the featurization stage</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Use this function in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>src/stage_02_featurization.py</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Write a function to create </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>artifacts/features</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> folder which will take the dir names from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>config.yml</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> file</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Stage 3 : </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">We will also create bag_of_words using CountVectorizer and Tfidf matrix </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(see NLP.xlsx for details)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.
+The purpose of this is that one single word not carry any meaning or context but group of words are meaningful.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> One important thing I would like to add here is both Tfidfvectorizer() and Tfidftransformer() perform the same calculation only difference is Tfidftransformer acts on sparse matrix (generated by CountVectorizer using raw text data) and Tfidfvectorizer acts directly on raw text data.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -701,6 +883,15 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1019,15 +1210,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:B44"/>
+  <dimension ref="B2:B54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="B34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="103.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="102.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
@@ -1077,32 +1268,32 @@
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="2:2" ht="75" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
@@ -1110,37 +1301,37 @@
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
@@ -1148,17 +1339,17 @@
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.25">
@@ -1166,62 +1357,110 @@
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B45" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B46" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B47" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B48" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="B49" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B50" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B53" s="2"/>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B54" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>